<commit_message>
additional changes to the plot
</commit_message>
<xml_diff>
--- a/apple2.xlsx
+++ b/apple2.xlsx
@@ -1455,7 +1455,7 @@
         <v>45729</v>
       </c>
       <c r="B51" t="n">
-        <v>211.8000030517578</v>
+        <v>211.8674011230469</v>
       </c>
       <c r="C51" t="n">
         <v>216.8394012451172</v>
@@ -1467,7 +1467,7 @@
         <v>215.9400024414062</v>
       </c>
       <c r="F51" t="n">
-        <v>39102506</v>
+        <v>39297750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Update to the course file
</commit_message>
<xml_diff>
--- a/apple2.xlsx
+++ b/apple2.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1447,7 +1447,7 @@
         <v>220.1399993896484</v>
       </c>
       <c r="F50" t="n">
-        <v>62466400</v>
+        <v>62547500</v>
       </c>
     </row>
     <row r="51">
@@ -1455,19 +1455,99 @@
         <v>45729</v>
       </c>
       <c r="B51" t="n">
-        <v>212.1000061035156</v>
+        <v>209.6799926757812</v>
       </c>
       <c r="C51" t="n">
-        <v>216.8394012451172</v>
+        <v>216.8399963378906</v>
       </c>
       <c r="D51" t="n">
-        <v>210.5001068115234</v>
+        <v>208.4199981689453</v>
       </c>
       <c r="E51" t="n">
-        <v>215.9400024414062</v>
+        <v>215.9499969482422</v>
       </c>
       <c r="F51" t="n">
-        <v>39427917</v>
+        <v>61368300</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45730</v>
+      </c>
+      <c r="B52" t="n">
+        <v>213.4900054931641</v>
+      </c>
+      <c r="C52" t="n">
+        <v>213.9499969482422</v>
+      </c>
+      <c r="D52" t="n">
+        <v>209.5800018310547</v>
+      </c>
+      <c r="E52" t="n">
+        <v>211.25</v>
+      </c>
+      <c r="F52" t="n">
+        <v>60107600</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45733</v>
+      </c>
+      <c r="B53" t="n">
+        <v>214</v>
+      </c>
+      <c r="C53" t="n">
+        <v>215.2200012207031</v>
+      </c>
+      <c r="D53" t="n">
+        <v>209.9700012207031</v>
+      </c>
+      <c r="E53" t="n">
+        <v>213.3099975585938</v>
+      </c>
+      <c r="F53" t="n">
+        <v>48073400</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>45734</v>
+      </c>
+      <c r="B54" t="n">
+        <v>212.6900024414062</v>
+      </c>
+      <c r="C54" t="n">
+        <v>215.1499938964844</v>
+      </c>
+      <c r="D54" t="n">
+        <v>211.4900054931641</v>
+      </c>
+      <c r="E54" t="n">
+        <v>214.1600036621094</v>
+      </c>
+      <c r="F54" t="n">
+        <v>42432400</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45735</v>
+      </c>
+      <c r="B55" t="n">
+        <v>215.2400054931641</v>
+      </c>
+      <c r="C55" t="n">
+        <v>218.7599945068359</v>
+      </c>
+      <c r="D55" t="n">
+        <v>213.75</v>
+      </c>
+      <c r="E55" t="n">
+        <v>214.2200012207031</v>
+      </c>
+      <c r="F55" t="n">
+        <v>54336700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>